<commit_message>
Added new tests. Refactored code.
</commit_message>
<xml_diff>
--- a/src/test/resources/testcases/TestScenarios_WebApi.xlsx
+++ b/src/test/resources/testcases/TestScenarios_WebApi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows User\Documents\Narendra\PersData\Testing Material\SoFiTechAssesment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC66D521-440C-4EE0-ADED-93AA20608194}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD16270-6796-4684-A435-791F8E1FDB85}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15210" xr2:uid="{8673CC63-9700-4F55-BDF7-5570500951CE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>TS Num.</t>
   </si>
@@ -61,11 +61,6 @@
 call should return "401 Unauthorized" with error message
 "status_code": 7,
 "status_message": "Invalid API key: You must be granted a valid key."</t>
-  </si>
-  <si>
-    <t>Can add more 
--Combination of tests. 
--Depending on detail understanding of requirements</t>
   </si>
   <si>
     <t>Verify that when GET Call "/movie/{movie_id}" executed with
@@ -108,14 +103,64 @@
   <si>
     <t>Verify that when GET Call "/movie/{movie_id}" executed with
 - Valid Movie ID with Leading And Trailing Spaces
+- With valid Language option (For e.g. French - "&amp;language=fr-FR") with Leading And Trailing Spaces
+call should get executed successfully with no error and response should return expected Movie details</t>
+  </si>
+  <si>
+    <t>Verify that when GET Call "/movie/{movie_id}" executed with
+- Valid Movie ID
 - With NO Language option mentioned (Should fall back to default US English)
 call should get executed successfully with no error and response should return expected Movie details (Should fall back to default US English)</t>
   </si>
   <si>
     <t>Verify that when GET Call "/movie/{movie_id}" executed with
 - Valid Movie ID
-- With INVALID Language option (For e.g.  "&amp;language=zz-ZZ") having Leading And Trailing Spaces
+- With INVALID/Non-Exist Language option (For e.g.  "&amp;language=zz-ZZ") 
 call should get executed successfully with no error and response should return expected Movie details (Should fall back to default US English)</t>
+  </si>
+  <si>
+    <t>Verify that when GET Call "/movie/{movie_id}" executed with
+- Missing/Null Movie ID
+call should return "404 Not Found" with error message
+"status_code": 34,
+"status_message": "The resource you requested could not be found."</t>
+  </si>
+  <si>
+    <t>Verify that when GET Call "/movie/{movie_id}" executed with
+-URL encoding prefix and suffix to Movie ID
+call should handle URL encoding as per expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that when GET Call "/movie/{movie_id}" executed with
+- Partial Movie ID
+call should get executed successfully 
+1) If Movie found  with exact match for Movie ID, return movie info
+2) If no Movie ID found matching exactly return
+{
+    "status_code": 34,
+    "status_message": "The resource you requested could not be found."
+}
+</t>
+  </si>
+  <si>
+    <t>TS-008</t>
+  </si>
+  <si>
+    <t>TS-009</t>
+  </si>
+  <si>
+    <t>TS-010</t>
+  </si>
+  <si>
+    <t>TS-011</t>
+  </si>
+  <si>
+    <t>TS-012</t>
+  </si>
+  <si>
+    <t>Verify that when GET Call "/movie/{movie_id}" executed with
+-URL encoding middle of Movie ID
+call should handle URL encoding as per expected</t>
   </si>
 </sst>
 </file>
@@ -153,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -176,48 +221,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
@@ -225,15 +233,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,7 +552,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,107 +574,135 @@
     </row>
     <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -783,9 +810,6 @@
       <c r="C34" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B9:B13"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>